<commit_message>
Chest resubmission analysis (cont.)
</commit_message>
<xml_diff>
--- a/Figures_Tables/result_tables/table2.xlsx
+++ b/Figures_Tables/result_tables/table2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="20860" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="5840" yWindow="380" windowWidth="20860" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+  <si>
+    <t>9.4 (+/-7.5)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.7 (+/-4.8)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 (0.76~1.42</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.44 (1.27~1.62)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1593 (+/-1476)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1759 (+/-1833)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>166 (-114~447)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blood Gas test count (per day)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>1 (+/-0.8)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -29,18 +61,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>-1.28 (-1.44~-1.11)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Venous Blood Gas test count (per day)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 (+/-0.9)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Primary Outcome</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -65,26 +85,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>-1.42 (-1.62~-1.24)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Total IV fluid volumn (1st day)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1564 (+/-1459)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1758 (+/-1852)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-0.12 (-0.27~-0.04)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>28 day mortality</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -105,10 +109,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>-0.66 (-0.82~-0.5)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;0.0001</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -117,18 +117,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>5.7 (+/-4.8)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>9.4 (+/-7.5)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-0.57 (-0.74~-0.41)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Ventilation time (surviors)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -141,11 +129,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>-0.54 (-0.7~-0.38)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Arterial Blood Gas test count (per day)</t>
+    <t>1.65 (1.24~2.07)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.47 (2.34~4.59)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -241,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -271,9 +259,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -606,10 +591,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -622,24 +607,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" thickTop="1">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6">
         <v>0.152</v>
@@ -648,7 +633,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="7">
         <v>0.83</v>
@@ -656,7 +641,7 @@
     </row>
     <row r="3" spans="1:5" ht="26">
       <c r="A3" s="8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -665,16 +650,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="11" t="s">
         <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -685,13 +670,13 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
@@ -699,16 +684,16 @@
     </row>
     <row r="6" spans="1:5" ht="26">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>22</v>
@@ -716,16 +701,16 @@
     </row>
     <row r="7" spans="1:5" ht="26">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>22</v>
@@ -733,35 +718,18 @@
     </row>
     <row r="8" spans="1:5" ht="26">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="26">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
         <v>0.24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final bag vbg study
</commit_message>
<xml_diff>
--- a/Figures_Tables/result_tables/table2.xlsx
+++ b/Figures_Tables/result_tables/table2.xlsx
@@ -19,7 +19,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+  <si>
+    <t>Venous Blood Gas test count (per day)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.017 (+/-0.1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.014 (+/-0.08)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.002 (-0.016~0.01)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>9.4 (+/-7.5)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -33,10 +49,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1.44 (1.27~1.62)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>1593 (+/-1476)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -49,15 +61,19 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Blood Gas test count (per day)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 (+/-0.8)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.4 (+/-1.4)</t>
+    <t>Arterial Blood Gas test count (per day)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8 (+/-0.7)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 (+/-1.2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4 (1.25~1.57)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -229,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -259,6 +275,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -591,11 +610,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -607,24 +624,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" thickTop="1">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" s="6">
         <v>0.152</v>
@@ -633,7 +650,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" s="7">
         <v>0.83</v>
@@ -641,7 +658,7 @@
     </row>
     <row r="3" spans="1:5" ht="26">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -650,90 +667,108 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="26">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="26">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="E8" s="1">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="26">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
         <v>0.24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>